<commit_message>
Multiple fixes: - Fixes in design and new features - New directory for all stylesheets
</commit_message>
<xml_diff>
--- a/backend/data/employees.xlsx
+++ b/backend/data/employees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MTC-hack\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F388FF-C48C-4432-B1D7-9775BDB5CB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09A111B-078F-48F9-9874-8B2DEFF39ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8070" yWindow="2655" windowWidth="20310" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="446">
   <si>
     <t>Подразделение 2</t>
   </si>
@@ -1694,8 +1694,8 @@
   </sheetPr>
   <dimension ref="A1:N1128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H198" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K218" sqref="K218"/>
+    <sheetView tabSelected="1" topLeftCell="C171" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1764,8 +1764,8 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
-        <v>0</v>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -1808,8 +1808,8 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -3128,8 +3128,8 @@
       <c r="C33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="1">
-        <v>0</v>
+      <c r="D33" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>42</v>
@@ -4668,8 +4668,8 @@
       <c r="C68" s="1">
         <v>0</v>
       </c>
-      <c r="D68" s="1">
-        <v>0</v>
+      <c r="D68" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>166</v>
@@ -4712,8 +4712,8 @@
       <c r="C69" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D69" s="1">
-        <v>0</v>
+      <c r="D69" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>166</v>
@@ -6296,8 +6296,8 @@
       <c r="C105" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D105" s="1">
-        <v>0</v>
+      <c r="D105" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>280</v>
@@ -6912,8 +6912,8 @@
       <c r="C119" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D119">
-        <v>0</v>
+      <c r="D119" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>280</v>
@@ -6956,8 +6956,8 @@
       <c r="C120" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D120">
-        <v>0</v>
+      <c r="D120" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>280</v>
@@ -7000,8 +7000,8 @@
       <c r="C121" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D121">
-        <v>0</v>
+      <c r="D121" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>280</v>
@@ -7044,8 +7044,8 @@
       <c r="C122" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D122">
-        <v>0</v>
+      <c r="D122" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>280</v>
@@ -7088,8 +7088,8 @@
       <c r="C123" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D123">
-        <v>0</v>
+      <c r="D123" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>280</v>
@@ -7132,8 +7132,8 @@
       <c r="C124" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D124">
-        <v>0</v>
+      <c r="D124" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>280</v>
@@ -7176,8 +7176,8 @@
       <c r="C125" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D125">
-        <v>0</v>
+      <c r="D125" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>280</v>
@@ -7220,8 +7220,8 @@
       <c r="C126" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D126">
-        <v>0</v>
+      <c r="D126" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>280</v>
@@ -7264,8 +7264,8 @@
       <c r="C127" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D127">
-        <v>0</v>
+      <c r="D127" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>280</v>
@@ -7308,8 +7308,8 @@
       <c r="C128" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D128">
-        <v>0</v>
+      <c r="D128" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>280</v>
@@ -7352,8 +7352,8 @@
       <c r="C129" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D129">
-        <v>0</v>
+      <c r="D129" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>280</v>
@@ -7396,8 +7396,8 @@
       <c r="C130" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D130">
-        <v>0</v>
+      <c r="D130" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>280</v>
@@ -7440,8 +7440,8 @@
       <c r="C131" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D131">
-        <v>0</v>
+      <c r="D131" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>280</v>
@@ -7484,8 +7484,8 @@
       <c r="C132" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D132">
-        <v>0</v>
+      <c r="D132" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>280</v>
@@ -7528,8 +7528,8 @@
       <c r="C133" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D133">
-        <v>0</v>
+      <c r="D133" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>280</v>
@@ -7572,8 +7572,8 @@
       <c r="C134" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D134">
-        <v>0</v>
+      <c r="D134" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>280</v>
@@ -7616,8 +7616,8 @@
       <c r="C135" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D135">
-        <v>0</v>
+      <c r="D135" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>280</v>
@@ -7660,8 +7660,8 @@
       <c r="C136" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D136">
-        <v>0</v>
+      <c r="D136" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>280</v>
@@ -7704,8 +7704,8 @@
       <c r="C137" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D137">
-        <v>0</v>
+      <c r="D137" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>280</v>
@@ -7748,8 +7748,8 @@
       <c r="C138" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D138">
-        <v>0</v>
+      <c r="D138" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>280</v>
@@ -7792,8 +7792,8 @@
       <c r="C139" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D139">
-        <v>0</v>
+      <c r="D139" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>280</v>
@@ -7836,8 +7836,8 @@
       <c r="C140" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D140">
-        <v>0</v>
+      <c r="D140" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>280</v>
@@ -7880,8 +7880,8 @@
       <c r="C141" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D141">
-        <v>0</v>
+      <c r="D141" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>280</v>
@@ -7924,8 +7924,8 @@
       <c r="C142" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D142">
-        <v>0</v>
+      <c r="D142" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>280</v>
@@ -7968,8 +7968,8 @@
       <c r="C143" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D143">
-        <v>0</v>
+      <c r="D143" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>280</v>
@@ -8012,8 +8012,8 @@
       <c r="C144" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D144">
-        <v>0</v>
+      <c r="D144" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>280</v>
@@ -8056,8 +8056,8 @@
       <c r="C145" s="1">
         <v>0</v>
       </c>
-      <c r="D145" s="1">
-        <v>0</v>
+      <c r="D145" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>280</v>
@@ -8100,8 +8100,8 @@
       <c r="C146" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D146" s="1">
-        <v>0</v>
+      <c r="D146" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>280</v>
@@ -9552,8 +9552,8 @@
       <c r="C179" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D179" s="1">
-        <v>0</v>
+      <c r="D179" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>280</v>
@@ -10124,8 +10124,8 @@
       <c r="C192" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D192">
-        <v>0</v>
+      <c r="D192" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>265</v>
@@ -10168,8 +10168,8 @@
       <c r="C193" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D193">
-        <v>0</v>
+      <c r="D193" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>265</v>
@@ -10212,8 +10212,8 @@
       <c r="C194" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D194">
-        <v>0</v>
+      <c r="D194" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>265</v>
@@ -10256,8 +10256,8 @@
       <c r="C195" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D195">
-        <v>0</v>
+      <c r="D195" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>265</v>
@@ -10300,8 +10300,8 @@
       <c r="C196" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D196">
-        <v>0</v>
+      <c r="D196" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>265</v>
@@ -10344,8 +10344,8 @@
       <c r="C197" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D197">
-        <v>0</v>
+      <c r="D197" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>265</v>
@@ -10388,8 +10388,8 @@
       <c r="C198" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D198">
-        <v>0</v>
+      <c r="D198" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>265</v>
@@ -10432,8 +10432,8 @@
       <c r="C199" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D199">
-        <v>0</v>
+      <c r="D199" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>280</v>
@@ -10476,8 +10476,8 @@
       <c r="C200" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D200">
-        <v>0</v>
+      <c r="D200" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>280</v>
@@ -10520,8 +10520,8 @@
       <c r="C201" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D201">
-        <v>0</v>
+      <c r="D201" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>280</v>
@@ -10564,8 +10564,8 @@
       <c r="C202" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D202">
-        <v>0</v>
+      <c r="D202" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>280</v>
@@ -10608,8 +10608,8 @@
       <c r="C203" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D203">
-        <v>0</v>
+      <c r="D203" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>280</v>
@@ -10652,8 +10652,8 @@
       <c r="C204" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D204">
-        <v>0</v>
+      <c r="D204" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>280</v>
@@ -10696,8 +10696,8 @@
       <c r="C205" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D205">
-        <v>0</v>
+      <c r="D205" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>42</v>
@@ -10740,8 +10740,8 @@
       <c r="C206" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D206">
-        <v>0</v>
+      <c r="D206" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>42</v>
@@ -10784,8 +10784,8 @@
       <c r="C207" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D207">
-        <v>0</v>
+      <c r="D207" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>42</v>
@@ -10828,8 +10828,8 @@
       <c r="C208" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D208">
-        <v>0</v>
+      <c r="D208" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>42</v>
@@ -10872,8 +10872,8 @@
       <c r="C209" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D209">
-        <v>0</v>
+      <c r="D209" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>42</v>
@@ -10916,8 +10916,8 @@
       <c r="C210" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D210">
-        <v>0</v>
+      <c r="D210" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>42</v>
@@ -10960,8 +10960,8 @@
       <c r="C211" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D211">
-        <v>0</v>
+      <c r="D211" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>42</v>
@@ -11004,8 +11004,8 @@
       <c r="C212" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D212">
-        <v>0</v>
+      <c r="D212" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>42</v>
@@ -11048,8 +11048,8 @@
       <c r="C213" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D213">
-        <v>0</v>
+      <c r="D213" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>42</v>
@@ -11092,8 +11092,8 @@
       <c r="C214" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D214">
-        <v>0</v>
+      <c r="D214" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>42</v>
@@ -11136,8 +11136,8 @@
       <c r="C215" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D215">
-        <v>0</v>
+      <c r="D215" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>42</v>
@@ -11180,7 +11180,7 @@
       <c r="C216">
         <v>0</v>
       </c>
-      <c r="D216">
+      <c r="D216" s="1">
         <v>0</v>
       </c>
       <c r="E216" s="1" t="s">

</xml_diff>